<commit_message>
merged data file of chem data for modeling
</commit_message>
<xml_diff>
--- a/Data/Processed Data/ICP/ICP_L1/Salinity_ICP_results_formatted.xlsx
+++ b/Data/Processed Data/ICP/ICP_L1/Salinity_ICP_results_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/tempest_ionic_strength/Data/Processed Data/ICP/ICP_L1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023A4164-6821-9946-8075-19F1F9A74BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A7EADC-6353-F644-802C-F8FFD65D3305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="760" windowWidth="29040" windowHeight="19840" xr2:uid="{99E1365F-92B2-41F8-9B0B-C669C816E218}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2229,7 +2229,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C36" s="2">
         <v>0.68100000000000005</v>

</xml_diff>